<commit_message>
hostnames to lower, projects to upper to avoid doubles and conflicts
</commit_message>
<xml_diff>
--- a/passwords.xlsx
+++ b/passwords.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t xml:space="preserve">project</t>
   </si>
@@ -32,6 +32,15 @@
   </si>
   <si>
     <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">masterdatas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testlower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testcamel</t>
   </si>
 </sst>
 </file>
@@ -173,10 +182,10 @@
   <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.3"/>
@@ -198,15 +207,32 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>

</xml_diff>